<commit_message>
Commit after major update and sharing draft with SAP
</commit_message>
<xml_diff>
--- a/data/NFHS5 Couples Variable List.xlsx
+++ b/data/NFHS5 Couples Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87900C30-1EDC-4664-9FBA-46BB757DCD01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFCBDC5-3CF0-4472-9362-AF235ED44D2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1944,19 +1944,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05E6B7D-B624-4BDD-B559-1E186C27DE33}">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="7.90625" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>467</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>219</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>221</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>223</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>225</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>227</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>229</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>231</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>206</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>237</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>239</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>242</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>245</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>250</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>256</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>131</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>135</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>137</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>139</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>140</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>99</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>176</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>277</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>285</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>287</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>475</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>476</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>477</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>478</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>479</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>488</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>489</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>498</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>492</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>499</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>495</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>504</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>506</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>510</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>511</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>104</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>105</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>106</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>107</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>204</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>172</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>298</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>171</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>111</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>119</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>120</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>22</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>23</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>305</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>309</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>313</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>316</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>14</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>17</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>19</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>338</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>20</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>21</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>346</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>24</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>25</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>27</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>28</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>29</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>30</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>371</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>209</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>518</v>
       </c>

</xml_diff>